<commit_message>
Info excel update & names models
</commit_message>
<xml_diff>
--- a/tareas_SOS.xlsx
+++ b/tareas_SOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\Desktop\tothexinxol\IRB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Enrique\Documents\GitHub\IRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5DA764-4642-4284-BDA2-69B8799D7435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23309E85-3841-4D62-ABBF-8E62D8B1D485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="303">
   <si>
     <t>TASKS</t>
   </si>
@@ -135,9 +135,6 @@
     <t>CYP3a4-substrate</t>
   </si>
   <si>
-    <t>TK_CYP3A4sub</t>
-  </si>
-  <si>
     <t>local: reimputed in linux server</t>
   </si>
   <si>
@@ -150,36 +147,24 @@
     <t>CYP2c9-subs</t>
   </si>
   <si>
-    <t>TK_CYP2C9sub</t>
-  </si>
-  <si>
     <t>CYP2C9</t>
   </si>
   <si>
     <t>CYP2c19-subs</t>
   </si>
   <si>
-    <t>TK_CYP2C19sub</t>
-  </si>
-  <si>
     <t>CYP2C19</t>
   </si>
   <si>
     <t>CYP1a2-sub</t>
   </si>
   <si>
-    <t>TK_CYP1A2sub</t>
-  </si>
-  <si>
     <t>CYP1A2</t>
   </si>
   <si>
     <t>CYP2d6-subs</t>
   </si>
   <si>
-    <t>TK_CYP2D6subs</t>
-  </si>
-  <si>
     <t>CYP2D6</t>
   </si>
   <si>
@@ -223,9 +208,6 @@
   </si>
   <si>
     <t>CYP2d6-inh</t>
-  </si>
-  <si>
-    <t>TK_CYP2D6inh</t>
   </si>
   <si>
     <t>TK_CYP2D6inh_DeepPK</t>
@@ -1014,9 +996,6 @@
     <t>Cav1.2inh</t>
   </si>
   <si>
-    <t>calculating descriptors</t>
-  </si>
-  <si>
     <t>TK_HIA_Wangdf1</t>
   </si>
   <si>
@@ -1078,6 +1057,39 @@
   </si>
   <si>
     <t>if needed, intermediate files folder inisde the model</t>
+  </si>
+  <si>
+    <t>ongoing: finetuning</t>
+  </si>
+  <si>
+    <t>TK_CYP2D6sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_CYP3A4sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_CYP2C19sub_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>TK_CYP2C9sub_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>TK_CYP1A2sub_NOoutliers</t>
+  </si>
+  <si>
+    <t>TK_CYP2D6inh_NOoutliers_us</t>
+  </si>
+  <si>
+    <t>CYP1A2_CYProduct.csv, CYP1A2_CYPstrate.csv, CYP1A2_Metrabase.csv, CYP1A2_Terri.csv, CYP1A2_Deep-PK.csv</t>
+  </si>
+  <si>
+    <t>CYP2D6_CYProduct.csv, CYP2D6_CYPstrate.csv, CYP2D6_Deep-PK.csv, CYP2D6_isoCYP.csv, CYP2D6_Magna.csv, CYP2D6_Metabase.csv, CYP2D6_Terri.csv</t>
+  </si>
+  <si>
+    <t>['Zaretzki, J., Rydberg, P., Bergeron, C., Bennett, K. P., Olsen, L., &amp; Breneman, C. M. (2012). RS-Predictor models augmented with SMARTCyp reactivities: Robust metabolic regioselectivity predictions for nine CYP isozymes. Journal of Chemical Information and Modeling, 52(6), 1637. https://doi.org/10.1021/CI300009Z.','Tyzack, J. D., Hunt, P. A., &amp; Segall, M. D. (2016). Predicting Regioselectivity and Lability of Cytochrome P450 Metabolism Using Quantum Mechanical Simulations. Journal of Chemical Information and Modeling, 56(11), 2180–2193. https://doi.org/10.1021/acs.jcim.6b00233.','Tian, S., Djoumbou-Feunang, Y., Greiner, R., &amp; Wishart, D. S. (2018). CypReact: A Software Tool for in Silico Reactant Prediction for Human Cytochrome P450 Enzymes. Journal of Chemical Information and Modeling, 58(6), 1282–1291. https://doi.org/10.1021/ACS.JCIM.8B00035/ASSET/IMAGES/MEDIUM/CI-2018-000356_0013.GIF.', 'de Bruyn Kops, C., Friedrich, N.-O., &amp; Kirchmair, J. (2017). Alignment-Based Prediction of Sites of Metabolism. Journal of Chemical Information and Modeling, 57(6), 1258–1264. https://doi.org/10.1021/acs.jcim.7b00165.', 'Manga, N., Duffy, J. C., Rowe, P. H., &amp; Cronin, M. T. D. (2005). Structure-Based Methods for the Prediction of the Dominant P450 Enzyme in Human Drug Biotransformation: Consideration of CYP3A4, CYP2C9, CYP2D6. SAR and QSAR in Environmental Research, 16(1–2), 43–61. https://doi.org/10.1080/10629360412331319871.', 'Terfloth, L., Bienfait, B., &amp; Gasteiger, J. (2007). Ligand-Based Models for the Isoform Specificity of Cytochrome P450 3A4, 2D6, and 2C9 Substrates. Journal of Chemical Information and Modeling, 47(4), 1688–1701. https://doi.org/10.1021/ci700010t.', 'Tian, S., Cao, X., Greiner, R., Li, C., Guo, A., &amp; Wishart, D. S. (2021). CyProduct: A Software Tool for Accurately Predicting the Byproducts of Human Cytochrome P450 Metabolism. Journal of Chemical Information and Modeling, 61(6), 3128–3140. https://doi.org/10.1021/acs.jcim.1c00144', 'Myung, Y., de Sá, A. G. C., &amp; Ascher, D. B. (2024). Deep-PK: deep learning for small molecule pharmacokinetic and toxicity prediction. Nucleic Acids Research, 52(W1), W469–W475. https://doi.org/10.1093/nar/gkae254.', 'https://www-metrabase.ch.cam.ac.uk/metrabaseui/?', ]</t>
+  </si>
+  <si>
+    <t>CYP1A2sub</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1159,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1178,6 +1190,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1191,7 +1209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1228,6 +1246,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,15 +1510,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="47.7109375" customWidth="1"/>
     <col min="6" max="6" width="34" customWidth="1"/>
@@ -1563,278 +1582,278 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="F6" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I6" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="E7" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I7" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="E8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I8" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>297</v>
       </c>
       <c r="E9" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>293</v>
       </c>
       <c r="E10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="H14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>45</v>
+        <v>39</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>298</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="7"/>
       <c r="H15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E16" s="14"/>
       <c r="F16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H16" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="H19" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>13</v>
@@ -1843,10 +1862,10 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>13</v>
@@ -1855,30 +1874,30 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G23" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>13</v>
@@ -1887,30 +1906,30 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="8" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F25" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="H25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>13</v>
@@ -1919,10 +1938,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D27" s="12" t="s">
         <v>13</v>
@@ -1931,128 +1950,128 @@
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="14" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E31" s="14"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F32" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="G32" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H32" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F33" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="G33" s="7"/>
       <c r="H33" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G34" s="7"/>
       <c r="H34" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="E36" s="14" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="F36" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2065,9 +2084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,1180 +2104,1183 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I1" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="J1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="M1" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" t="s">
-        <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I1" s="15" t="s">
-        <v>281</v>
-      </c>
-      <c r="J1" t="s">
-        <v>298</v>
-      </c>
-      <c r="K1" t="s">
-        <v>112</v>
-      </c>
-      <c r="L1" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="M2" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
         <v>115</v>
       </c>
-      <c r="B3" t="s">
+      <c r="G3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" t="s">
-        <v>121</v>
-      </c>
-      <c r="G3" t="s">
-        <v>122</v>
-      </c>
       <c r="I3" s="15" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="M3" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="L4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="M4" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K5" t="s">
+        <v>127</v>
+      </c>
+      <c r="L5" t="s">
         <v>128</v>
       </c>
-      <c r="C5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" t="s">
-        <v>131</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K5" t="s">
-        <v>133</v>
-      </c>
-      <c r="L5" t="s">
-        <v>134</v>
-      </c>
       <c r="M5" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G6" t="s">
+        <v>130</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K6" t="s">
+        <v>131</v>
+      </c>
+      <c r="L6" t="s">
         <v>128</v>
       </c>
-      <c r="C6" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" t="s">
-        <v>136</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K6" t="s">
-        <v>137</v>
-      </c>
-      <c r="L6" t="s">
-        <v>134</v>
-      </c>
       <c r="M6" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" t="s">
+        <v>124</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K7" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7" t="s">
         <v>128</v>
       </c>
-      <c r="C7" t="s">
-        <v>138</v>
-      </c>
-      <c r="D7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" t="s">
-        <v>139</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K7" t="s">
-        <v>140</v>
-      </c>
-      <c r="L7" t="s">
-        <v>134</v>
-      </c>
       <c r="M7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L8" t="s">
         <v>128</v>
       </c>
-      <c r="C8" t="s">
-        <v>141</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K8" t="s">
-        <v>143</v>
-      </c>
-      <c r="L8" t="s">
-        <v>134</v>
-      </c>
       <c r="M8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" t="s">
+        <v>124</v>
+      </c>
+      <c r="G9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K9" t="s">
+        <v>140</v>
+      </c>
+      <c r="L9" t="s">
         <v>128</v>
       </c>
-      <c r="C9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K9" t="s">
-        <v>146</v>
-      </c>
-      <c r="L9" t="s">
-        <v>134</v>
-      </c>
       <c r="M9" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" t="s">
+        <v>142</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" t="s">
         <v>128</v>
       </c>
-      <c r="C10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F10" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10" t="s">
-        <v>148</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" t="s">
-        <v>149</v>
-      </c>
-      <c r="L10" t="s">
-        <v>134</v>
-      </c>
       <c r="M10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" t="s">
+        <v>144</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" t="s">
+        <v>145</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" t="s">
+        <v>146</v>
+      </c>
+      <c r="L11" t="s">
         <v>128</v>
       </c>
-      <c r="C11" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-      <c r="F11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" t="s">
-        <v>151</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="K11" t="s">
-        <v>152</v>
-      </c>
-      <c r="L11" t="s">
-        <v>134</v>
-      </c>
       <c r="M11" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B12" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="M12" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="K14" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="L14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="M14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="K15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="L15" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="M15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F16" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="K16" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="L16" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="M16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B17" t="s">
         <v>165</v>
       </c>
-      <c r="B17" t="s">
-        <v>171</v>
-      </c>
       <c r="C17" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="G17" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I17" s="15" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="M17" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C18" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F18" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I18" s="15" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="K18" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="L18" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M18" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B19" t="s">
         <v>175</v>
       </c>
-      <c r="B19" t="s">
-        <v>181</v>
-      </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" t="s">
+        <v>124</v>
+      </c>
+      <c r="G19" t="s">
+        <v>161</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="K19" t="s">
         <v>177</v>
       </c>
-      <c r="E19" t="s">
-        <v>178</v>
-      </c>
-      <c r="F19" t="s">
-        <v>130</v>
-      </c>
-      <c r="G19" t="s">
-        <v>167</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>182</v>
-      </c>
-      <c r="K19" t="s">
-        <v>183</v>
-      </c>
       <c r="L19" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M19" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B20" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E20" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F20" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I20" s="15" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="K20" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="L20" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M20" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F21" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G21" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I21" s="15" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K21" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="L21" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M21" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D22" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E22" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K22" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="L22" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M22" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G23" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G24" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G25" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" s="15" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C28" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G28" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="K28" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M28" s="17"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="C29" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D29" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
+        <v>188</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" t="s">
         <v>194</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" t="s">
-        <v>200</v>
-      </c>
       <c r="I29" s="15" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J29" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K29" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M29" s="17"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C30" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G30" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="I30" s="15" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="K30" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="L30" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M30" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G31" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I31" s="15" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="J31" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K31" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="L31" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M31" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C32" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="D32" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E32" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="J32" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="K32" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="L32" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M32" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="D33" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E33" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G33" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I33" s="15" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="K33" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="L33" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="M33" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D34" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E34" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G34" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="I34" s="15" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="K34" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="L34" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="M34" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D35" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B36" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="C36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G36" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="I36" s="15" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="L36" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M36" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B37" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G37" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="I37" s="15" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="L37" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M37" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B38" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G38" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="I38" s="15" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="L38" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="M38" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B39" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D39" s="6"/>
       <c r="G39" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="I39" s="15" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
       <c r="L39" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>227</v>
+      </c>
       <c r="C40" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D40" s="6"/>
       <c r="G40" t="s">
-        <v>234</v>
+        <v>301</v>
       </c>
       <c r="I40" s="15" t="s">
-        <v>234</v>
+        <v>300</v>
       </c>
       <c r="L40" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E41" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G41" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I41" s="15" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="K41" s="15" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="M41" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B42" s="16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="D42" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G42" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I42" s="15" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="M42" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D43" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F43" s="11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="G43" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="I43" s="15" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="K43" s="15" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="M43" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -3290,10 +3312,10 @@
   <sheetData>
     <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3301,66 +3323,66 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="B4" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="C7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3381,17 +3403,17 @@
   <sheetData>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -3399,32 +3421,32 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
@@ -3432,147 +3454,147 @@
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
last updates and ramiro predictions
</commit_message>
<xml_diff>
--- a/tareas_SOS.xlsx
+++ b/tareas_SOS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\Desktop\tothexinxol\IRB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741641C4-6C63-44F8-8ABD-0C72B659CE74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA39924-EC11-497B-8CF8-09A8E4C7080E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="23280" windowHeight="12600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="legend" sheetId="3" r:id="rId3"/>
     <sheet name="propuesta_inicial" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -33,7 +33,7 @@
     <author>Autoría desconocida</author>
   </authors>
   <commentList>
-    <comment ref="L29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="L30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="L31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="306">
   <si>
     <t>TASKS</t>
   </si>
@@ -1086,6 +1086,15 @@
   </si>
   <si>
     <t>TK_Caco2</t>
+  </si>
+  <si>
+    <t>TK_HLM_Li</t>
+  </si>
+  <si>
+    <t>https://pubs.acs.org/doi/abs/10.1021/acs.jcim.5b00255</t>
+  </si>
+  <si>
+    <t>TK_HLM_vnnADMET discarded. TK_HLM_Li</t>
   </si>
 </sst>
 </file>
@@ -1153,7 +1162,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1190,6 +1199,12 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79979857783745845"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1203,7 +1218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1241,6 +1256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,7 +1521,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1781,7 +1797,7 @@
         <v>52</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>305</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -2097,11 +2113,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6:L11"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,71 +2499,62 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" t="s">
+        <v>303</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" t="s">
+        <v>304</v>
+      </c>
+      <c r="I13" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F14" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G14" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="I13" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L14" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M14" s="8" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>118</v>
-      </c>
-      <c r="B14" t="s">
-        <v>164</v>
-      </c>
-      <c r="C14" t="s">
-        <v>56</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" t="s">
-        <v>134</v>
-      </c>
-      <c r="G14" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>165</v>
-      </c>
-      <c r="K14" t="s">
-        <v>166</v>
-      </c>
-      <c r="L14" t="s">
-        <v>130</v>
-      </c>
-      <c r="M14" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -2555,10 +2562,10 @@
         <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>52</v>
@@ -2573,10 +2580,10 @@
         <v>128</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K15" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="L15" t="s">
         <v>130</v>
@@ -2587,13 +2594,13 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B16" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
       <c r="D16" t="s">
         <v>52</v>
@@ -2605,16 +2612,16 @@
         <v>134</v>
       </c>
       <c r="G16" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="K16" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="L16" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="M16" t="s">
         <v>131</v>
@@ -2628,7 +2635,7 @@
         <v>171</v>
       </c>
       <c r="C17" t="s">
-        <v>295</v>
+        <v>91</v>
       </c>
       <c r="D17" t="s">
         <v>52</v>
@@ -2640,13 +2647,19 @@
         <v>134</v>
       </c>
       <c r="G17" t="s">
-        <v>296</v>
+        <v>172</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>297</v>
+        <v>173</v>
+      </c>
+      <c r="K17" t="s">
+        <v>174</v>
       </c>
       <c r="L17" t="s">
-        <v>258</v>
+        <v>175</v>
+      </c>
+      <c r="M17" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -2654,54 +2667,48 @@
         <v>170</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C18" t="s">
-        <v>177</v>
+        <v>295</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>134</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>296</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="M18" t="s">
-        <v>179</v>
+        <v>297</v>
+      </c>
+      <c r="L18" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>118</v>
+        <v>170</v>
       </c>
       <c r="B19" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>181</v>
-      </c>
-      <c r="F19" t="s">
-        <v>134</v>
+        <v>177</v>
       </c>
       <c r="G19" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="K19" t="s">
-        <v>183</v>
-      </c>
-      <c r="L19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="M19" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -2709,10 +2716,10 @@
         <v>118</v>
       </c>
       <c r="B20" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
@@ -2727,10 +2734,10 @@
         <v>172</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="K20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="L20" t="s">
         <v>184</v>
@@ -2744,10 +2751,10 @@
         <v>118</v>
       </c>
       <c r="B21" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>64</v>
@@ -2762,10 +2769,10 @@
         <v>172</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K21" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="L21" t="s">
         <v>184</v>
@@ -2779,10 +2786,10 @@
         <v>118</v>
       </c>
       <c r="B22" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
         <v>64</v>
@@ -2797,10 +2804,10 @@
         <v>172</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="K22" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="L22" t="s">
         <v>184</v>
@@ -2814,10 +2821,10 @@
         <v>118</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
@@ -2832,10 +2839,10 @@
         <v>172</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="K23" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="L23" t="s">
         <v>184</v>
@@ -2845,8 +2852,38 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="G24" s="14" t="s">
-        <v>163</v>
+      <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" t="s">
+        <v>181</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>172</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="K24" t="s">
+        <v>196</v>
+      </c>
+      <c r="L24" t="s">
+        <v>184</v>
+      </c>
+      <c r="M24" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -2864,38 +2901,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>170</v>
-      </c>
-      <c r="B29" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="C29" t="s">
-        <v>198</v>
-      </c>
-      <c r="D29" t="s">
-        <v>84</v>
-      </c>
-      <c r="E29" t="s">
-        <v>199</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" t="s">
-        <v>200</v>
-      </c>
-      <c r="I29" s="14" t="s">
-        <v>201</v>
-      </c>
-      <c r="K29" t="s">
-        <v>202</v>
-      </c>
-      <c r="L29" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="M29" s="8"/>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G28" s="14" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -2905,7 +2914,7 @@
         <v>197</v>
       </c>
       <c r="C30" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D30" t="s">
         <v>84</v>
@@ -2917,16 +2926,13 @@
         <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I30" s="14" t="s">
-        <v>205</v>
-      </c>
-      <c r="J30" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="K30" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L30" s="15" t="s">
         <v>184</v>
@@ -2938,10 +2944,10 @@
         <v>170</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C31" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="D31" t="s">
         <v>84</v>
@@ -2953,20 +2959,21 @@
         <v>134</v>
       </c>
       <c r="G31" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="I31" s="14" t="s">
-        <v>211</v>
+        <v>205</v>
+      </c>
+      <c r="J31" t="s">
+        <v>206</v>
       </c>
       <c r="K31" t="s">
-        <v>212</v>
-      </c>
-      <c r="L31" t="s">
+        <v>207</v>
+      </c>
+      <c r="L31" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="M31" t="s">
-        <v>131</v>
-      </c>
+      <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2976,7 +2983,7 @@
         <v>208</v>
       </c>
       <c r="C32" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D32" t="s">
         <v>84</v>
@@ -2988,16 +2995,13 @@
         <v>134</v>
       </c>
       <c r="G32" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I32" s="14" t="s">
-        <v>215</v>
-      </c>
-      <c r="J32" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K32" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L32" t="s">
         <v>184</v>
@@ -3011,10 +3015,10 @@
         <v>170</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C33" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D33" t="s">
         <v>84</v>
@@ -3026,16 +3030,16 @@
         <v>134</v>
       </c>
       <c r="G33" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I33" s="14" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J33" t="s">
         <v>206</v>
       </c>
       <c r="K33" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="L33" t="s">
         <v>184</v>
@@ -3052,7 +3056,7 @@
         <v>217</v>
       </c>
       <c r="C34" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D34" t="s">
         <v>84</v>
@@ -3064,13 +3068,16 @@
         <v>134</v>
       </c>
       <c r="G34" t="s">
-        <v>172</v>
+        <v>219</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>223</v>
+        <v>220</v>
+      </c>
+      <c r="J34" t="s">
+        <v>206</v>
       </c>
       <c r="K34" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L34" t="s">
         <v>184</v>
@@ -3086,11 +3093,11 @@
       <c r="B35" s="14" t="s">
         <v>217</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>225</v>
+      <c r="C35" t="s">
+        <v>222</v>
       </c>
       <c r="D35" t="s">
-        <v>52</v>
+        <v>84</v>
       </c>
       <c r="E35" t="s">
         <v>199</v>
@@ -3099,74 +3106,86 @@
         <v>134</v>
       </c>
       <c r="G35" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K35" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L35" t="s">
-        <v>227</v>
+        <v>184</v>
       </c>
       <c r="M35" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="s">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>170</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>52</v>
+      <c r="E36" t="s">
+        <v>199</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G36" t="s">
+        <v>157</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="K36" t="s">
+        <v>226</v>
+      </c>
+      <c r="L36" t="s">
+        <v>227</v>
+      </c>
+      <c r="M36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" t="s">
-        <v>228</v>
-      </c>
-      <c r="C37" t="s">
-        <v>17</v>
-      </c>
-      <c r="G37" t="s">
-        <v>229</v>
-      </c>
-      <c r="I37" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="L37" t="s">
-        <v>231</v>
-      </c>
-      <c r="M37" t="s">
-        <v>232</v>
-      </c>
+      <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>118</v>
       </c>
       <c r="B38" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G38" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="L38" t="s">
         <v>231</v>
@@ -3180,16 +3199,16 @@
         <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G39" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="L39" t="s">
         <v>231</v>
@@ -3203,20 +3222,22 @@
         <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>239</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>236</v>
+      </c>
+      <c r="C40" t="s">
+        <v>24</v>
+      </c>
       <c r="G40" t="s">
         <v>237</v>
       </c>
       <c r="I40" s="14" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="L40" t="s">
         <v>231</v>
+      </c>
+      <c r="M40" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -3224,52 +3245,41 @@
         <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D41" s="1"/>
       <c r="G41" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="I41" s="14" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="L41" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="D42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E42" t="s">
-        <v>52</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="B42" t="s">
+        <v>241</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="1"/>
       <c r="G42" t="s">
-        <v>163</v>
+        <v>242</v>
       </c>
       <c r="I42" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="K42" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="M42" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="L42" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -3280,7 +3290,7 @@
         <v>72</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="D43" t="s">
         <v>64</v>
@@ -3298,10 +3308,10 @@
         <v>162</v>
       </c>
       <c r="K43" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="M43" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -3312,7 +3322,7 @@
         <v>72</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D44" t="s">
         <v>64</v>
@@ -3330,25 +3340,57 @@
         <v>162</v>
       </c>
       <c r="K44" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="M44" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>250</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>52</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G45" t="s">
+        <v>163</v>
+      </c>
+      <c r="I45" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="K45" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="M44" t="s">
+      <c r="M45" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>170</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G46" t="s">
         <v>253</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G30" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G31" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="G32" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="G31" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G32" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="G33" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>